<commit_message>
feat: "finding nodes for tmp when reaching threshold by dfs (non-general)"
</commit_message>
<xml_diff>
--- a/exercise2/data.xlsx
+++ b/exercise2/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,13 +436,162 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>nodes</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>penalty of flows</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>demand of nodes</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>(1,2, p = 15, c = 500)</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(1,4, p = 17, c = 200)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>17</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(2,3, p = 8, c = 100)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>(2,5, p = 7, c = 133)</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>(3,6, p = 12, c = 100)</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(4,5, p = 15, c = 700)</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>15</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>(4,7, p = 1, c = 500)</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>(5,6, p = 5, c = 200)</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>(5,8, p = 7, c = 500)</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>